<commit_message>
create funcs and load trs
</commit_message>
<xml_diff>
--- a/data/map.xlsx
+++ b/data/map.xlsx
@@ -72,7 +72,7 @@
     <t>Survey</t>
   </si>
   <si>
-    <t>SE/4 SW/4 S32 7N 1E, S5 6N 1E</t>
+    <t>S5 6N 1E, S32 7N 1E, SE/4 SW/4 S32 7N 1E</t>
   </si>
 </sst>
 </file>
@@ -394,7 +394,7 @@
   <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="A7:XFD7"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
add parcel and tract numbers and add page number to scan
</commit_message>
<xml_diff>
--- a/data/map.xlsx
+++ b/data/map.xlsx
@@ -66,13 +66,13 @@
     <t>Record Map</t>
   </si>
   <si>
-    <t>NO MAP</t>
-  </si>
-  <si>
     <t>Survey</t>
   </si>
   <si>
     <t>S5 6N 1E, S32 7N 1E, SE/4 SW/4 S32 7N 1E</t>
+  </si>
+  <si>
+    <t>NO MAP ON FILE</t>
   </si>
 </sst>
 </file>
@@ -466,7 +466,7 @@
         <v>13</v>
       </c>
       <c r="I2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -483,7 +483,7 @@
         <v>1</v>
       </c>
       <c r="H3" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -500,7 +500,7 @@
         <v>1</v>
       </c>
       <c r="H4" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -517,12 +517,12 @@
         <v>1</v>
       </c>
       <c r="H5" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B6">
         <v>5</v>
@@ -534,7 +534,7 @@
         <v>1</v>
       </c>
       <c r="H6" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update61 + add surveyor fullname check
</commit_message>
<xml_diff>
--- a/data/map.xlsx
+++ b/data/map.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18625"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18730"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="20">
   <si>
     <t>MAPTYPE</t>
   </si>
@@ -73,6 +73,12 @@
   </si>
   <si>
     <t>NO MAP ON FILE</t>
+  </si>
+  <si>
+    <t>TEST GRID (TR1)</t>
+  </si>
+  <si>
+    <t>TEST GRID</t>
   </si>
 </sst>
 </file>
@@ -391,10 +397,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -537,6 +543,26 @@
         <v>17</v>
       </c>
     </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7">
+        <v>99</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="G7" t="s">
+        <v>18</v>
+      </c>
+      <c r="H7" t="s">
+        <v>19</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>